<commit_message>
20250426 12:54  Add a copy of the license and modify the profile
</commit_message>
<xml_diff>
--- a/메이플스토리.xlsx
+++ b/메이플스토리.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="현재_통합_문서" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{395BC90E-DF4A-4131-A91C-DEFB38764421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{182EC7AF-09AA-44AB-990F-8751D8447AB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28965" yWindow="120" windowWidth="23670" windowHeight="16680" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29085" yWindow="1725" windowWidth="21600" windowHeight="15150" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="계정" sheetId="3" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="344">
   <si>
     <t>이름</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1342,6 +1342,10 @@
   </si>
   <si>
     <t>루미너스M</t>
+  </si>
+  <si>
+    <t>K전사카이저</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1660,6 +1664,9 @@
     <xf numFmtId="41" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="41" fontId="5" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1669,9 +1676,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="5" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="백분율" xfId="2" builtinId="5"/>
@@ -1680,80 +1684,6 @@
     <cellStyle name="하이퍼링크" xfId="3" builtinId="8"/>
   </cellStyles>
   <dxfs count="55">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -1848,6 +1778,80 @@
       <font>
         <color rgb="FFFF0000"/>
       </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -2361,10 +2365,10 @@
       <c r="D3" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="28" t="s">
         <v>213</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="28" t="s">
         <v>266</v>
       </c>
     </row>
@@ -2376,8 +2380,8 @@
       <c r="D4" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B5" s="9"/>
@@ -2387,8 +2391,8 @@
       <c r="D5" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B7" s="9" t="s">
@@ -2560,7 +2564,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C42" sqref="C42"/>
+      <selection pane="bottomRight" activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -2586,9 +2590,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="C1" s="30">
+      <c r="C1" s="27">
         <f>C2-32</f>
-        <v>7827</v>
+        <v>7994</v>
       </c>
       <c r="L1" s="1">
         <f>COLUMN()-9</f>
@@ -2630,11 +2634,11 @@
     <row r="2" spans="1:24" x14ac:dyDescent="0.15">
       <c r="B2" s="1">
         <f>COUNTIF(B$5:B$55,"*" &amp; B3 &amp; "*")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="26">
         <f>C3+캐릭터m!C3</f>
-        <v>7859</v>
+        <v>8026</v>
       </c>
       <c r="D2" s="1">
         <f>COUNTIF(D$5:D$55,"*" &amp; D3 &amp; "*")</f>
@@ -2659,7 +2663,7 @@
       </c>
       <c r="C3" s="15">
         <f>SUM(C5:C55)-136</f>
-        <v>7718</v>
+        <v>7885</v>
       </c>
       <c r="D3" t="s">
         <v>221</v>
@@ -2848,7 +2852,7 @@
       </c>
       <c r="X6" s="2">
         <f>COUNTIF($E$5:$E$55,V6)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.15">
@@ -3921,7 +3925,7 @@
       </c>
       <c r="X19" s="2">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.15">
@@ -5616,7 +5620,7 @@
         <v>312</v>
       </c>
       <c r="C42" s="2">
-        <v>123</v>
+        <v>172</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>15</v>
@@ -5689,21 +5693,25 @@
         <v>39</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
+        <v>343</v>
+      </c>
+      <c r="C43" s="2">
+        <v>118</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="E43" s="2" t="str">
         <f>IF(D43="","",VLOOKUP($D43,직업!$B$3:$D$524,2,FALSE))</f>
-        <v/>
+        <v>전사</v>
       </c>
       <c r="F43" s="2">
         <f t="shared" ref="F43:F54" si="7">IFERROR(VLOOKUP(E43,$V$6:$W$11,2,FALSE),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G43" s="2" t="str">
         <f>IF(OR(E43="",RIGHT(D43,1)="M"),"",VLOOKUP($D43,직업!$B$3:$D$524,3,FALSE))</f>
-        <v/>
+        <v>노바</v>
       </c>
       <c r="H43" s="2">
         <f>IFERROR(VLOOKUP(B43,배치!$B$4:$I$55,7,FALSE),"")</f>
@@ -5712,19 +5720,19 @@
       <c r="I43" s="3"/>
       <c r="J43" s="2">
         <f t="shared" ref="J43:J54" si="8">IFERROR(VLOOKUP(G43,$V$14:$W$24,2,FALSE),0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K43" s="3" t="str">
         <f>IF(J43=0,"",VLOOKUP(J43,$J$5:T42,2,FALSE))</f>
-        <v/>
+        <v>산호</v>
       </c>
       <c r="L43" s="3" t="str">
         <f>IF($K43="","",IFERROR(IF(VLOOKUP($J43,$J$5:T42,L$1,FALSE)="","",VLOOKUP($J43,$J$5:T42,L$1,FALSE)),""))</f>
-        <v/>
+        <v>나리</v>
       </c>
       <c r="M43" s="3" t="str">
         <f>IF($K43="","",IFERROR(IF(VLOOKUP($J43,$J$5:U42,M$1,FALSE)="","",VLOOKUP($J43,$J$5:U42,M$1,FALSE)),""))</f>
-        <v/>
+        <v>백호</v>
       </c>
       <c r="N43" s="3" t="str">
         <f>IF($K43="","",IFERROR(IF(VLOOKUP($J43,$J$5:V42,N$1,FALSE)="","",VLOOKUP($J43,$J$5:V42,N$1,FALSE)),""))</f>
@@ -6655,7 +6663,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -6843,46 +6851,16 @@
       <c r="J5" s="2">
         <v>2</v>
       </c>
-      <c r="K5" s="3" t="str">
-        <f ca="1">IFERROR(VLOOKUP(J5,$J4:T$5,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="L5" s="3" t="str">
-        <f ca="1">IF($K5="","",IFERROR(IF(VLOOKUP($J5,$J4:T$5,L$1,FALSE)="","",VLOOKUP($J5,$J4:T$5,L$1,FALSE)),""))</f>
-        <v/>
-      </c>
-      <c r="M5" s="3" t="str">
-        <f ca="1">IF($K5="","",IFERROR(IF(VLOOKUP($J5,$J4:U$5,M$1,FALSE)="","",VLOOKUP($J5,$J4:U$5,M$1,FALSE)),""))</f>
-        <v/>
-      </c>
-      <c r="N5" s="3" t="str">
-        <f ca="1">IF($K5="","",IFERROR(IF(VLOOKUP($J5,$J4:V$5,N$1,FALSE)="","",VLOOKUP($J5,$J4:V$5,N$1,FALSE)),""))</f>
-        <v/>
-      </c>
-      <c r="O5" s="3" t="str">
-        <f ca="1">IF($K5="","",IFERROR(IF(VLOOKUP($J5,$J4:W$5,O$1,FALSE)="","",VLOOKUP($J5,$J4:W$5,O$1,FALSE)),""))</f>
-        <v/>
-      </c>
-      <c r="P5" s="3" t="str">
-        <f ca="1">IF($K5="","",IFERROR(IF(VLOOKUP($J5,$J4:X$5,P$1,FALSE)="","",VLOOKUP($J5,$J4:X$5,P$1,FALSE)),""))</f>
-        <v/>
-      </c>
-      <c r="Q5" s="3" t="str">
-        <f ca="1">IF($K5="","",IFERROR(IF(VLOOKUP($J5,$J4:Y$5,Q$1,FALSE)="","",VLOOKUP($J5,$J4:Y$5,Q$1,FALSE)),""))</f>
-        <v/>
-      </c>
-      <c r="R5" s="3" t="str">
-        <f ca="1">IF($K5="","",IFERROR(IF(VLOOKUP($J5,$J4:Z$5,R$1,FALSE)="","",VLOOKUP($J5,$J4:Z$5,R$1,FALSE)),""))</f>
-        <v/>
-      </c>
-      <c r="S5" s="3" t="str">
-        <f ca="1">IF($K5="","",IFERROR(IF(VLOOKUP($J5,$J4:AA$5,S$1,FALSE)="","",VLOOKUP($J5,$J4:AA$5,S$1,FALSE)),""))</f>
-        <v/>
-      </c>
-      <c r="T5" s="3" t="str">
-        <f ca="1">IF($K5="","",IFERROR(IF(VLOOKUP($J5,$J4:AB$5,T$1,FALSE)="","",VLOOKUP($J5,$J4:AB$5,T$1,FALSE)),""))</f>
-        <v/>
-      </c>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
       <c r="V5" s="4" t="s">
         <v>340</v>
       </c>
@@ -6928,44 +6906,44 @@
         <f t="shared" ref="J6:J54" si="3">IFERROR(VLOOKUP(G6,$V$14:$W$24,2,FALSE),0)</f>
         <v>2</v>
       </c>
-      <c r="K6" s="3" t="str">
-        <f ca="1">IFERROR(VLOOKUP(J6,$J$5:T5,2,FALSE),"")</f>
-        <v/>
+      <c r="K6" s="3">
+        <f>IFERROR(VLOOKUP(J6,$J$5:T5,2,FALSE),"")</f>
+        <v>0</v>
       </c>
       <c r="L6" s="3" t="str">
-        <f ca="1">IF($K6="","",IFERROR(IF(VLOOKUP($J6,$J$5:T5,L$1,FALSE)="","",VLOOKUP($J6,$J$5:T5,L$1,FALSE)),""))</f>
+        <f>IF($K6="","",IFERROR(IF(VLOOKUP($J6,$J$5:T5,L$1,FALSE)="","",VLOOKUP($J6,$J$5:T5,L$1,FALSE)),""))</f>
         <v/>
       </c>
       <c r="M6" s="3" t="str">
-        <f ca="1">IF($K6="","",IFERROR(IF(VLOOKUP($J6,$J$5:U5,M$1,FALSE)="","",VLOOKUP($J6,$J$5:U5,M$1,FALSE)),""))</f>
+        <f>IF($K6="","",IFERROR(IF(VLOOKUP($J6,$J$5:U5,M$1,FALSE)="","",VLOOKUP($J6,$J$5:U5,M$1,FALSE)),""))</f>
         <v/>
       </c>
       <c r="N6" s="3" t="str">
-        <f ca="1">IF($K6="","",IFERROR(IF(VLOOKUP($J6,$J$5:V5,N$1,FALSE)="","",VLOOKUP($J6,$J$5:V5,N$1,FALSE)),""))</f>
+        <f>IF($K6="","",IFERROR(IF(VLOOKUP($J6,$J$5:V5,N$1,FALSE)="","",VLOOKUP($J6,$J$5:V5,N$1,FALSE)),""))</f>
         <v/>
       </c>
       <c r="O6" s="3" t="str">
-        <f ca="1">IF($K6="","",IFERROR(IF(VLOOKUP($J6,$J$5:W5,O$1,FALSE)="","",VLOOKUP($J6,$J$5:W5,O$1,FALSE)),""))</f>
+        <f>IF($K6="","",IFERROR(IF(VLOOKUP($J6,$J$5:W5,O$1,FALSE)="","",VLOOKUP($J6,$J$5:W5,O$1,FALSE)),""))</f>
         <v/>
       </c>
       <c r="P6" s="3" t="str">
-        <f ca="1">IF($K6="","",IFERROR(IF(VLOOKUP($J6,$J$5:X5,P$1,FALSE)="","",VLOOKUP($J6,$J$5:X5,P$1,FALSE)),""))</f>
+        <f>IF($K6="","",IFERROR(IF(VLOOKUP($J6,$J$5:X5,P$1,FALSE)="","",VLOOKUP($J6,$J$5:X5,P$1,FALSE)),""))</f>
         <v/>
       </c>
       <c r="Q6" s="3" t="str">
-        <f ca="1">IF($K6="","",IFERROR(IF(VLOOKUP($J6,$J$5:Y5,Q$1,FALSE)="","",VLOOKUP($J6,$J$5:Y5,Q$1,FALSE)),""))</f>
+        <f>IF($K6="","",IFERROR(IF(VLOOKUP($J6,$J$5:Y5,Q$1,FALSE)="","",VLOOKUP($J6,$J$5:Y5,Q$1,FALSE)),""))</f>
         <v/>
       </c>
       <c r="R6" s="3" t="str">
-        <f ca="1">IF($K6="","",IFERROR(IF(VLOOKUP($J6,$J$5:Z5,R$1,FALSE)="","",VLOOKUP($J6,$J$5:Z5,R$1,FALSE)),""))</f>
+        <f>IF($K6="","",IFERROR(IF(VLOOKUP($J6,$J$5:Z5,R$1,FALSE)="","",VLOOKUP($J6,$J$5:Z5,R$1,FALSE)),""))</f>
         <v/>
       </c>
       <c r="S6" s="3" t="str">
-        <f ca="1">IF($K6="","",IFERROR(IF(VLOOKUP($J6,$J$5:AA5,S$1,FALSE)="","",VLOOKUP($J6,$J$5:AA5,S$1,FALSE)),""))</f>
+        <f>IF($K6="","",IFERROR(IF(VLOOKUP($J6,$J$5:AA5,S$1,FALSE)="","",VLOOKUP($J6,$J$5:AA5,S$1,FALSE)),""))</f>
         <v/>
       </c>
       <c r="T6" s="3" t="str">
-        <f ca="1">IF($K6="","",IFERROR(IF(VLOOKUP($J6,$J$5:AB5,T$1,FALSE)="","",VLOOKUP($J6,$J$5:AB5,T$1,FALSE)),""))</f>
+        <f>IF($K6="","",IFERROR(IF(VLOOKUP($J6,$J$5:AB5,T$1,FALSE)="","",VLOOKUP($J6,$J$5:AB5,T$1,FALSE)),""))</f>
         <v/>
       </c>
       <c r="V6" s="3" t="s">
@@ -7014,44 +6992,44 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="K7" s="3" t="str">
-        <f ca="1">IFERROR(VLOOKUP(J7,$J$5:T6,2,FALSE),"")</f>
-        <v/>
+      <c r="K7" s="3">
+        <f>IFERROR(VLOOKUP(J7,$J$5:T6,2,FALSE),"")</f>
+        <v>0</v>
       </c>
       <c r="L7" s="3" t="str">
-        <f ca="1">IF($K7="","",IFERROR(IF(VLOOKUP($J7,$J$5:T6,L$1,FALSE)="","",VLOOKUP($J7,$J$5:T6,L$1,FALSE)),""))</f>
+        <f>IF($K7="","",IFERROR(IF(VLOOKUP($J7,$J$5:T6,L$1,FALSE)="","",VLOOKUP($J7,$J$5:T6,L$1,FALSE)),""))</f>
         <v/>
       </c>
       <c r="M7" s="3" t="str">
-        <f ca="1">IF($K7="","",IFERROR(IF(VLOOKUP($J7,$J$5:U6,M$1,FALSE)="","",VLOOKUP($J7,$J$5:U6,M$1,FALSE)),""))</f>
+        <f>IF($K7="","",IFERROR(IF(VLOOKUP($J7,$J$5:U6,M$1,FALSE)="","",VLOOKUP($J7,$J$5:U6,M$1,FALSE)),""))</f>
         <v/>
       </c>
       <c r="N7" s="3" t="str">
-        <f ca="1">IF($K7="","",IFERROR(IF(VLOOKUP($J7,$J$5:V6,N$1,FALSE)="","",VLOOKUP($J7,$J$5:V6,N$1,FALSE)),""))</f>
+        <f>IF($K7="","",IFERROR(IF(VLOOKUP($J7,$J$5:V6,N$1,FALSE)="","",VLOOKUP($J7,$J$5:V6,N$1,FALSE)),""))</f>
         <v/>
       </c>
       <c r="O7" s="3" t="str">
-        <f ca="1">IF($K7="","",IFERROR(IF(VLOOKUP($J7,$J$5:W6,O$1,FALSE)="","",VLOOKUP($J7,$J$5:W6,O$1,FALSE)),""))</f>
+        <f>IF($K7="","",IFERROR(IF(VLOOKUP($J7,$J$5:W6,O$1,FALSE)="","",VLOOKUP($J7,$J$5:W6,O$1,FALSE)),""))</f>
         <v/>
       </c>
       <c r="P7" s="3" t="str">
-        <f ca="1">IF($K7="","",IFERROR(IF(VLOOKUP($J7,$J$5:X6,P$1,FALSE)="","",VLOOKUP($J7,$J$5:X6,P$1,FALSE)),""))</f>
+        <f>IF($K7="","",IFERROR(IF(VLOOKUP($J7,$J$5:X6,P$1,FALSE)="","",VLOOKUP($J7,$J$5:X6,P$1,FALSE)),""))</f>
         <v/>
       </c>
       <c r="Q7" s="3" t="str">
-        <f ca="1">IF($K7="","",IFERROR(IF(VLOOKUP($J7,$J$5:Y6,Q$1,FALSE)="","",VLOOKUP($J7,$J$5:Y6,Q$1,FALSE)),""))</f>
+        <f>IF($K7="","",IFERROR(IF(VLOOKUP($J7,$J$5:Y6,Q$1,FALSE)="","",VLOOKUP($J7,$J$5:Y6,Q$1,FALSE)),""))</f>
         <v/>
       </c>
       <c r="R7" s="3" t="str">
-        <f ca="1">IF($K7="","",IFERROR(IF(VLOOKUP($J7,$J$5:Z6,R$1,FALSE)="","",VLOOKUP($J7,$J$5:Z6,R$1,FALSE)),""))</f>
+        <f>IF($K7="","",IFERROR(IF(VLOOKUP($J7,$J$5:Z6,R$1,FALSE)="","",VLOOKUP($J7,$J$5:Z6,R$1,FALSE)),""))</f>
         <v/>
       </c>
       <c r="S7" s="3" t="str">
-        <f ca="1">IF($K7="","",IFERROR(IF(VLOOKUP($J7,$J$5:AA6,S$1,FALSE)="","",VLOOKUP($J7,$J$5:AA6,S$1,FALSE)),""))</f>
+        <f>IF($K7="","",IFERROR(IF(VLOOKUP($J7,$J$5:AA6,S$1,FALSE)="","",VLOOKUP($J7,$J$5:AA6,S$1,FALSE)),""))</f>
         <v/>
       </c>
       <c r="T7" s="3" t="str">
-        <f ca="1">IF($K7="","",IFERROR(IF(VLOOKUP($J7,$J$5:AB6,T$1,FALSE)="","",VLOOKUP($J7,$J$5:AB6,T$1,FALSE)),""))</f>
+        <f>IF($K7="","",IFERROR(IF(VLOOKUP($J7,$J$5:AB6,T$1,FALSE)="","",VLOOKUP($J7,$J$5:AB6,T$1,FALSE)),""))</f>
         <v/>
       </c>
       <c r="V7" s="3" t="s">
@@ -7100,44 +7078,44 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="K8" s="3" t="str">
-        <f ca="1">IFERROR(VLOOKUP(J8,$J$5:T7,2,FALSE),"")</f>
-        <v/>
+      <c r="K8" s="3">
+        <f>IFERROR(VLOOKUP(J8,$J$5:T7,2,FALSE),"")</f>
+        <v>0</v>
       </c>
       <c r="L8" s="3" t="str">
-        <f ca="1">IF($K8="","",IFERROR(IF(VLOOKUP($J8,$J$5:T7,L$1,FALSE)="","",VLOOKUP($J8,$J$5:T7,L$1,FALSE)),""))</f>
+        <f>IF($K8="","",IFERROR(IF(VLOOKUP($J8,$J$5:T7,L$1,FALSE)="","",VLOOKUP($J8,$J$5:T7,L$1,FALSE)),""))</f>
         <v/>
       </c>
       <c r="M8" s="3" t="str">
-        <f ca="1">IF($K8="","",IFERROR(IF(VLOOKUP($J8,$J$5:U7,M$1,FALSE)="","",VLOOKUP($J8,$J$5:U7,M$1,FALSE)),""))</f>
+        <f>IF($K8="","",IFERROR(IF(VLOOKUP($J8,$J$5:U7,M$1,FALSE)="","",VLOOKUP($J8,$J$5:U7,M$1,FALSE)),""))</f>
         <v/>
       </c>
       <c r="N8" s="3" t="str">
-        <f ca="1">IF($K8="","",IFERROR(IF(VLOOKUP($J8,$J$5:V7,N$1,FALSE)="","",VLOOKUP($J8,$J$5:V7,N$1,FALSE)),""))</f>
+        <f>IF($K8="","",IFERROR(IF(VLOOKUP($J8,$J$5:V7,N$1,FALSE)="","",VLOOKUP($J8,$J$5:V7,N$1,FALSE)),""))</f>
         <v/>
       </c>
       <c r="O8" s="3" t="str">
-        <f ca="1">IF($K8="","",IFERROR(IF(VLOOKUP($J8,$J$5:W7,O$1,FALSE)="","",VLOOKUP($J8,$J$5:W7,O$1,FALSE)),""))</f>
+        <f>IF($K8="","",IFERROR(IF(VLOOKUP($J8,$J$5:W7,O$1,FALSE)="","",VLOOKUP($J8,$J$5:W7,O$1,FALSE)),""))</f>
         <v/>
       </c>
       <c r="P8" s="3" t="str">
-        <f ca="1">IF($K8="","",IFERROR(IF(VLOOKUP($J8,$J$5:X7,P$1,FALSE)="","",VLOOKUP($J8,$J$5:X7,P$1,FALSE)),""))</f>
+        <f>IF($K8="","",IFERROR(IF(VLOOKUP($J8,$J$5:X7,P$1,FALSE)="","",VLOOKUP($J8,$J$5:X7,P$1,FALSE)),""))</f>
         <v/>
       </c>
       <c r="Q8" s="3" t="str">
-        <f ca="1">IF($K8="","",IFERROR(IF(VLOOKUP($J8,$J$5:Y7,Q$1,FALSE)="","",VLOOKUP($J8,$J$5:Y7,Q$1,FALSE)),""))</f>
+        <f>IF($K8="","",IFERROR(IF(VLOOKUP($J8,$J$5:Y7,Q$1,FALSE)="","",VLOOKUP($J8,$J$5:Y7,Q$1,FALSE)),""))</f>
         <v/>
       </c>
       <c r="R8" s="3" t="str">
-        <f ca="1">IF($K8="","",IFERROR(IF(VLOOKUP($J8,$J$5:Z7,R$1,FALSE)="","",VLOOKUP($J8,$J$5:Z7,R$1,FALSE)),""))</f>
+        <f>IF($K8="","",IFERROR(IF(VLOOKUP($J8,$J$5:Z7,R$1,FALSE)="","",VLOOKUP($J8,$J$5:Z7,R$1,FALSE)),""))</f>
         <v/>
       </c>
       <c r="S8" s="3" t="str">
-        <f ca="1">IF($K8="","",IFERROR(IF(VLOOKUP($J8,$J$5:AA7,S$1,FALSE)="","",VLOOKUP($J8,$J$5:AA7,S$1,FALSE)),""))</f>
+        <f>IF($K8="","",IFERROR(IF(VLOOKUP($J8,$J$5:AA7,S$1,FALSE)="","",VLOOKUP($J8,$J$5:AA7,S$1,FALSE)),""))</f>
         <v/>
       </c>
       <c r="T8" s="3" t="str">
-        <f ca="1">IF($K8="","",IFERROR(IF(VLOOKUP($J8,$J$5:AB7,T$1,FALSE)="","",VLOOKUP($J8,$J$5:AB7,T$1,FALSE)),""))</f>
+        <f>IF($K8="","",IFERROR(IF(VLOOKUP($J8,$J$5:AB7,T$1,FALSE)="","",VLOOKUP($J8,$J$5:AB7,T$1,FALSE)),""))</f>
         <v/>
       </c>
       <c r="V8" s="3" t="s">
@@ -10753,7 +10731,7 @@
       </c>
       <c r="I5" s="2">
         <f>COUNTIF(캐릭터!$E$4:$E$55,G5)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.15">
@@ -10974,7 +10952,7 @@
       </c>
       <c r="E13" s="2">
         <f>COUNTIF(캐릭터!$D$4:$D$55,$B13)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>11</v>
@@ -11105,7 +11083,7 @@
       </c>
       <c r="I17" s="2">
         <f>COUNTIF(캐릭터!$G$4:$G$55,G17)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.15">
@@ -13202,27 +13180,27 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="E4:E16 E18:E22 E24:E63">
-    <cfRule type="cellIs" dxfId="11" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="14" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="expression" dxfId="10" priority="13">
+    <cfRule type="expression" dxfId="27" priority="13">
       <formula>AND(ISBLANK($B$2)=FALSE,FIND($B$2,B17))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E17">
-    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="12" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23">
-    <cfRule type="expression" dxfId="8" priority="11">
+    <cfRule type="expression" dxfId="25" priority="11">
       <formula>AND(ISBLANK($B$2)=FALSE,FIND($B$2,B23))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
-    <cfRule type="cellIs" dxfId="7" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="10" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13239,7 +13217,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:I10">
-    <cfRule type="expression" dxfId="6" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="2" stopIfTrue="1">
       <formula>$H5=$I5</formula>
     </cfRule>
     <cfRule type="colorScale" priority="8">
@@ -13254,32 +13232,32 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:B63 D4:D63">
-    <cfRule type="expression" dxfId="5" priority="7">
+    <cfRule type="expression" dxfId="22" priority="7">
       <formula>AND(ISBLANK(B$2)=FALSE,ISBLANK(B4)=FALSE,FIND(B$2,B4))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D17">
-    <cfRule type="expression" dxfId="4" priority="6">
+    <cfRule type="expression" dxfId="21" priority="6">
       <formula>AND(ISBLANK($B$2)=FALSE,FIND($B$2,D17))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23">
-    <cfRule type="expression" dxfId="3" priority="5">
+    <cfRule type="expression" dxfId="20" priority="5">
       <formula>AND(ISBLANK($B$2)=FALSE,FIND($B$2,D23))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:H10">
-    <cfRule type="expression" dxfId="2" priority="4">
+    <cfRule type="expression" dxfId="19" priority="4">
       <formula>$H5=$I5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12:H28">
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="18" priority="3">
       <formula>$H12=$I12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12:I28">
-    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="1" stopIfTrue="1">
       <formula>$H12=$I12</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13340,7 +13318,7 @@
       </c>
       <c r="C3" s="12">
         <f>SUM(C5:C55)-136</f>
-        <v>7718</v>
+        <v>7885</v>
       </c>
       <c r="D3" t="s">
         <v>54</v>
@@ -14753,7 +14731,7 @@
       </c>
       <c r="C42" s="2">
         <f>캐릭터!C42</f>
-        <v>123</v>
+        <v>172</v>
       </c>
       <c r="D42" s="3" t="str">
         <f>캐릭터!D42</f>
@@ -14784,27 +14762,27 @@
       </c>
       <c r="B43" s="3" t="str">
         <f>캐릭터!B43</f>
-        <v>K</v>
+        <v>K전사카이저</v>
       </c>
       <c r="C43" s="2">
         <f>캐릭터!C43</f>
-        <v>0</v>
-      </c>
-      <c r="D43" s="3">
+        <v>118</v>
+      </c>
+      <c r="D43" s="3" t="str">
         <f>캐릭터!D43</f>
-        <v>0</v>
+        <v>카이저</v>
       </c>
       <c r="E43" s="3" t="str">
         <f>캐릭터!E43</f>
-        <v/>
+        <v>전사</v>
       </c>
       <c r="F43" s="2">
         <f>캐릭터!F43</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G43" s="3" t="str">
         <f>캐릭터!G43</f>
-        <v/>
+        <v>노바</v>
       </c>
       <c r="H43" s="2"/>
       <c r="I43" s="3" t="str">
@@ -15211,37 +15189,37 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B4:B55">
-    <cfRule type="expression" dxfId="28" priority="7">
+    <cfRule type="expression" dxfId="16" priority="7">
       <formula>AND(ISBLANK(B$3)=FALSE,FIND(B$3,B4))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:G55">
-    <cfRule type="expression" dxfId="27" priority="4">
+    <cfRule type="expression" dxfId="15" priority="4">
       <formula>AND(ISBLANK(G$3)=FALSE,FIND(G$3,G4))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:D55">
-    <cfRule type="expression" dxfId="26" priority="6">
+    <cfRule type="expression" dxfId="14" priority="6">
       <formula>AND(ISBLANK(D$3)=FALSE,FIND(D$3,D4))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:E55">
-    <cfRule type="expression" dxfId="25" priority="5">
+    <cfRule type="expression" dxfId="13" priority="5">
       <formula>AND(ISBLANK(E$3)=FALSE,FIND(E$3,E4))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:H54">
-    <cfRule type="expression" dxfId="24" priority="3">
+    <cfRule type="expression" dxfId="12" priority="3">
       <formula>$H5=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:I55">
-    <cfRule type="expression" dxfId="23" priority="2">
+    <cfRule type="expression" dxfId="11" priority="2">
       <formula>AND(ISBLANK(I$3)=FALSE,FIND(I$3,I4))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:I54">
-    <cfRule type="expression" dxfId="22" priority="1">
+    <cfRule type="expression" dxfId="10" priority="1">
       <formula>$H5=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16013,22 +15991,22 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="A4:A57">
-    <cfRule type="expression" dxfId="21" priority="4">
+    <cfRule type="expression" dxfId="9" priority="4">
       <formula>AND(ISBLANK(A$3)=FALSE,FIND(A$3,A4))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:D57">
-    <cfRule type="expression" dxfId="20" priority="1">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>AND(ISBLANK(D$3)=FALSE,FIND(D$3,D4))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:B57">
-    <cfRule type="expression" dxfId="19" priority="3">
+    <cfRule type="expression" dxfId="7" priority="3">
       <formula>AND(ISBLANK(B$3)=FALSE,FIND(B$3,B4))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:C57">
-    <cfRule type="expression" dxfId="18" priority="2">
+    <cfRule type="expression" dxfId="6" priority="2">
       <formula>AND(ISBLANK(C$3)=FALSE,FIND(C$3,C4))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16489,10 +16467,10 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="H5:H10">
-    <cfRule type="cellIs" dxfId="17" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="6" stopIfTrue="1" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="9" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="9" stopIfTrue="1" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
     <cfRule type="colorScale" priority="10">
@@ -16507,10 +16485,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H14:H19">
-    <cfRule type="cellIs" dxfId="15" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" stopIfTrue="1" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="5" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="5" stopIfTrue="1" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
     <cfRule type="colorScale" priority="7">
@@ -16525,10 +16503,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H23:H31">
-    <cfRule type="cellIs" dxfId="13" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="2" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="2" stopIfTrue="1" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
     <cfRule type="colorScale" priority="3">

</xml_diff>